<commit_message>
save before migrating to project folder
</commit_message>
<xml_diff>
--- a/Ancillary Files/Site_List.xlsx
+++ b/Ancillary Files/Site_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\2022_County_LowFlow\Ancillary Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7BD722-D959-463C-AE71-45CB75495319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E998D2E4-ABCC-478F-988B-0707A4BD6654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Site_List" sheetId="1" r:id="rId1"/>

</xml_diff>